<commit_message>
Added handling for null location values
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -920,6 +920,46 @@
         </is>
       </c>
     </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Full Stack Engineer</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>- Git: All code is in Git.
+- Go: Services are written in Go.
+- SQL: Extensive use of SQL with both Postgres and duckDB.
+- AWS: Use of AWS, but architecture remains cloud agnostic.
+- Svelte: Frontends are written in Svelte with JS and SCSS.
+- JavaScript: Frontends are written in Svelte with JS and SCSS.
+- SCSS: Frontends are written in Svelte with JS and SCSS.
+- Swift: Sprinkle of Swift for native where low level device access is needed.
+- Java: Sprinkle of Java for native where low level device access is needed.</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>No specific degree or years of experience are explicitly required, but a "can-do attitude and the curiosity to ask questions" are emphasized.</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>https://www.linkedin.com/jobs/collections/recommended/?currentJobId=4168233573</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>4168233573</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>Payd</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>